<commit_message>
Vision changes in java code and python code
-not yet merged with the python cleanup
-untested
</commit_message>
<xml_diff>
--- a/Vision/Vision Testing Data.xlsx
+++ b/Vision/Vision Testing Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="9555" windowHeight="7230" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="9555" windowHeight="7230" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Height (Pixels)</t>
   </si>
@@ -38,6 +37,9 @@
   </si>
   <si>
     <t>Adjusted Angle</t>
+  </si>
+  <si>
+    <t>Distance From Goal</t>
   </si>
 </sst>
 </file>
@@ -374,11 +376,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47592960"/>
-        <c:axId val="47594496"/>
+        <c:axId val="146999936"/>
+        <c:axId val="147001728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47592960"/>
+        <c:axId val="146999936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,12 +390,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47594496"/>
+        <c:crossAx val="147001728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47594496"/>
+        <c:axId val="147001728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,7 +406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47592960"/>
+        <c:crossAx val="146999936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -614,11 +616,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153477120"/>
-        <c:axId val="153012480"/>
+        <c:axId val="147044224"/>
+        <c:axId val="147045760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153477120"/>
+        <c:axId val="147044224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,12 +630,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153012480"/>
+        <c:crossAx val="147045760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153012480"/>
+        <c:axId val="147045760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +646,285 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153477120"/>
+        <c:crossAx val="147044224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal Angle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>19.290046219188735</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.250505507133241</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.629377730656817</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.56505117707799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.256437163529263</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.992020198558663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41.185925165709648</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49.398705354995535</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.255118703057782</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>74.054604099077153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Angle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.999996219188731</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.96045550713324</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.339327730656819</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52.275001177077989</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55.966387163529262</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.701970198558662</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>66.89587516570964</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75.108655354995534</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85.965068703057781</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99.764554099077145</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="70469120"/>
+        <c:axId val="70467584"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="70469120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70467584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="70467584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70469120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -715,6 +995,41 @@
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1023,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,9 +1349,10 @@
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1047,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -1058,7 +1374,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.5</v>
       </c>
@@ -1069,7 +1385,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1080,7 +1396,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.5</v>
       </c>
@@ -1091,7 +1407,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -1101,8 +1417,11 @@
       <c r="C6">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7.5</v>
       </c>
@@ -1112,8 +1431,15 @@
       <c r="C7">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>140</v>
+      </c>
+      <c r="P7">
+        <f>44.139*EXP(-0.012*O7)</f>
+        <v>8.2263609284035173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1124,7 +1450,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.5</v>
       </c>
@@ -1135,7 +1461,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1146,7 +1472,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9.5</v>
       </c>
@@ -1157,7 +1483,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1168,7 +1494,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10.5</v>
       </c>
@@ -1179,7 +1505,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1190,7 +1516,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11.5</v>
       </c>
@@ -1201,7 +1527,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1420,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,7 +1812,7 @@
         <v>22</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D3:D5" si="0">C4+A4</f>
+        <f t="shared" ref="D4:D5" si="0">C4+A4</f>
         <v>37</v>
       </c>
     </row>
@@ -1513,12 +1839,172 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <f>DEGREES(ATAN(7/A2))</f>
+        <v>19.290046219188735</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>25.709953780811265</v>
+      </c>
+      <c r="E2">
+        <f>B2+25.70995</f>
+        <v>44.999996219188731</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B23" si="0">DEGREES(ATAN(7/A3))</f>
+        <v>21.250505507133241</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E11" si="1">B3+25.70995</f>
+        <v>46.96045550713324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>23.629377730656817</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>49.339327730656819</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>26.56505117707799</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>52.275001177077989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>30.256437163529263</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>55.966387163529262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>34.992020198558663</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>60.701970198558662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>41.185925165709648</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>66.89587516570964</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>49.398705354995535</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>75.108655354995534</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>60.255118703057782</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>85.965068703057781</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>74.054604099077153</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>99.764554099077145</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Changes for UNH
This works, go back to it if we break stuff
</commit_message>
<xml_diff>
--- a/Vision/Vision Testing Data.xlsx
+++ b/Vision/Vision Testing Data.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhsfirst\Documents\GitHub\frc-2016\Vision\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9555" windowHeight="7230" activeTab="2"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -87,6 +92,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -376,37 +384,75 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="146999936"/>
-        <c:axId val="147001728"/>
+        <c:axId val="269742984"/>
+        <c:axId val="269743768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="146999936"/>
+        <c:axId val="269742984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Target Width (Pixels)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147001728"/>
+        <c:crossAx val="269743768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147001728"/>
+        <c:axId val="269743768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance from Target (feet)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146999936"/>
+        <c:crossAx val="269742984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -616,11 +662,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147044224"/>
-        <c:axId val="147045760"/>
+        <c:axId val="269744160"/>
+        <c:axId val="269747688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147044224"/>
+        <c:axId val="269744160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,12 +676,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147045760"/>
+        <c:crossAx val="269747688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147045760"/>
+        <c:axId val="269747688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,7 +692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147044224"/>
+        <c:crossAx val="269744160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -894,11 +940,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="70469120"/>
-        <c:axId val="70467584"/>
+        <c:axId val="269747296"/>
+        <c:axId val="269748080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70469120"/>
+        <c:axId val="269747296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -908,12 +954,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70467584"/>
+        <c:crossAx val="269748080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70467584"/>
+        <c:axId val="269748080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,7 +970,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70469120"/>
+        <c:crossAx val="269747296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1094,7 +1140,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1129,7 +1175,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1340,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,7 +1888,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,7 +1937,7 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B23" si="0">DEGREES(ATAN(7/A3))</f>
+        <f t="shared" ref="B3:B11" si="0">DEGREES(ATAN(7/A3))</f>
         <v>21.250505507133241</v>
       </c>
       <c r="E3">

</xml_diff>

<commit_message>
Vision Changes from Pine Tree
</commit_message>
<xml_diff>
--- a/Vision/Vision Testing Data.xlsx
+++ b/Vision/Vision Testing Data.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhsfirst\Documents\GitHub\frc-2016\Vision\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9555" windowHeight="7230" activeTab="2"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -92,9 +87,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -384,75 +376,37 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="269742984"/>
-        <c:axId val="269743768"/>
+        <c:axId val="146999936"/>
+        <c:axId val="147001728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="269742984"/>
+        <c:axId val="146999936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Target Width (Pixels)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269743768"/>
+        <c:crossAx val="147001728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="269743768"/>
+        <c:axId val="147001728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Distance from Target (feet)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269742984"/>
+        <c:crossAx val="146999936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -662,11 +616,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="269744160"/>
-        <c:axId val="269747688"/>
+        <c:axId val="147044224"/>
+        <c:axId val="147045760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="269744160"/>
+        <c:axId val="147044224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,12 +630,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269747688"/>
+        <c:crossAx val="147045760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="269747688"/>
+        <c:axId val="147045760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,7 +646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269744160"/>
+        <c:crossAx val="147044224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -940,11 +894,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="269747296"/>
-        <c:axId val="269748080"/>
+        <c:axId val="70469120"/>
+        <c:axId val="70467584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="269747296"/>
+        <c:axId val="70469120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,12 +908,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269748080"/>
+        <c:crossAx val="70467584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="269748080"/>
+        <c:axId val="70467584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -970,7 +924,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269747296"/>
+        <c:crossAx val="70469120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1140,7 +1094,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1175,7 +1129,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1386,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,7 +1842,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1891,7 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B11" si="0">DEGREES(ATAN(7/A3))</f>
+        <f t="shared" ref="B3:B23" si="0">DEGREES(ATAN(7/A3))</f>
         <v>21.250505507133241</v>
       </c>
       <c r="E3">

</xml_diff>

<commit_message>
Cherry picked changes from #52
vision2016Testing.py literally didn't run, and these changes removed the
code that enabled it to work with opencv 3 (and setup document)
</commit_message>
<xml_diff>
--- a/Vision/Vision Testing Data.xlsx
+++ b/Vision/Vision Testing Data.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhsfirst\Documents\GitHub\frc-2016\Vision\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9555" windowHeight="7230" activeTab="2"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -92,9 +87,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -384,75 +376,37 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="269742984"/>
-        <c:axId val="269743768"/>
+        <c:axId val="146999936"/>
+        <c:axId val="147001728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="269742984"/>
+        <c:axId val="146999936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Target Width (Pixels)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269743768"/>
+        <c:crossAx val="147001728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="269743768"/>
+        <c:axId val="147001728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Distance from Target (feet)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269742984"/>
+        <c:crossAx val="146999936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -662,11 +616,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="269744160"/>
-        <c:axId val="269747688"/>
+        <c:axId val="147044224"/>
+        <c:axId val="147045760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="269744160"/>
+        <c:axId val="147044224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,12 +630,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269747688"/>
+        <c:crossAx val="147045760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="269747688"/>
+        <c:axId val="147045760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,7 +646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269744160"/>
+        <c:crossAx val="147044224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -940,11 +894,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="269747296"/>
-        <c:axId val="269748080"/>
+        <c:axId val="70469120"/>
+        <c:axId val="70467584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="269747296"/>
+        <c:axId val="70469120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,12 +908,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269748080"/>
+        <c:crossAx val="70467584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="269748080"/>
+        <c:axId val="70467584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -970,7 +924,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269747296"/>
+        <c:crossAx val="70469120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1140,7 +1094,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1175,7 +1129,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1386,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,7 +1842,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1891,7 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B11" si="0">DEGREES(ATAN(7/A3))</f>
+        <f t="shared" ref="B3:B23" si="0">DEGREES(ATAN(7/A3))</f>
         <v>21.250505507133241</v>
       </c>
       <c r="E3">

</xml_diff>